<commit_message>
Updates based on previous test results.
Search was updated to resolve a case sensitivity issue that was preventing search from functioning correctly. Search now functions as expected.
All forms updated to only accept numbers in ID, Year, and Ratings fields.
Add, update, and delete movie functions will no longer accept blank user input.
Delete movie will no longer delete a movie from the list when given a value that is not in the array.

All test cases have been resolved.
</commit_message>
<xml_diff>
--- a/UIFunctionTest.xlsx
+++ b/UIFunctionTest.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentbhtafeedu-my.sharepoint.com/personal/s10168314_student_bhtafe_edu_au/Documents/Cert 4 Programming/ICTICT449 Javascript/Assessments/JSAT2/Part5/JS-AT2-Part5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="252" documentId="13_ncr:1_{44B9C5A5-A56F-4E35-831E-6153A7234269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54A11AB8-A009-4009-AACE-1AE75CEFF439}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="13_ncr:1_{44B9C5A5-A56F-4E35-831E-6153A7234269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3774A8AE-DF91-4ADD-917F-ED4EEA5B31C3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case ID 01" sheetId="10" r:id="rId1"/>
+    <sheet name="Test Case ID 02" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="78">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -243,9 +244,6 @@
     <t>button is clickable by the user and the movie list is updated as expected.</t>
   </si>
   <si>
-    <t>Form did not accept the user input. No movie was added.</t>
-  </si>
-  <si>
     <t>A movie with invalid data is added to the list.</t>
   </si>
   <si>
@@ -258,13 +256,40 @@
     <t>No movie data is changed.</t>
   </si>
   <si>
-    <t>The movie at the bottom of the list deleted.</t>
-  </si>
-  <si>
     <t>Rob Hodgskiss</t>
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>button is clickable by the user, and the movie list will update to display only movies containing the search string.</t>
+  </si>
+  <si>
+    <t>With partial data entered in the Add a movie form, click the Add a movie button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID: 1234
+Title: 
+Year: 2000
+Rating: </t>
+  </si>
+  <si>
+    <t>Form will not accept the user input. No movie was updated.</t>
+  </si>
+  <si>
+    <t>Form will not accept the user input. No movie was added.</t>
+  </si>
+  <si>
+    <t>button is clickable by the user, and the movie list is not updated.</t>
+  </si>
+  <si>
+    <t>No movie was deleted from the list.</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>The movie at the bottom of the list was deleted.</t>
   </si>
 </sst>
 </file>
@@ -347,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +387,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -492,6 +523,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -501,35 +541,74 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
@@ -541,61 +620,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -885,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883A4F42-1B46-4B1E-B91B-251F58B3FD09}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -908,27 +948,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="32">
+      <c r="B1" s="17"/>
+      <c r="C1" s="27">
         <v>1</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="36" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="25" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="2"/>
@@ -946,73 +986,73 @@
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="38" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="28">
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="21">
         <v>45827</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="30" t="s">
+      <c r="I3" s="22"/>
+      <c r="J3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" s="41"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="26"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="17" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="20" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="17" t="s">
+      <c r="G5" s="37"/>
+      <c r="H5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="17" t="s">
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A7" s="3">
@@ -1030,16 +1070,16 @@
         <v>14</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="8"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="11"/>
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A8" s="3">
@@ -1057,16 +1097,16 @@
         <v>16</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="11" t="s">
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="10"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A9" s="3">
@@ -1084,16 +1124,16 @@
         <v>45</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8"/>
+      <c r="H9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A10" s="3">
@@ -1111,16 +1151,16 @@
         <v>25</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="8"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A11" s="3">
@@ -1138,97 +1178,97 @@
         <v>20</v>
       </c>
       <c r="G11" s="5"/>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="8"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A12" s="3">
         <v>6</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="9" t="s">
+      <c r="E12" s="15"/>
+      <c r="F12" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="6" t="s">
+      <c r="G12" s="15"/>
+      <c r="H12" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="15"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="39"/>
+      <c r="M12" s="40"/>
     </row>
     <row r="13" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A13" s="3">
         <v>7</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="15"/>
+      <c r="F13" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="6" t="s">
+      <c r="G13" s="15"/>
+      <c r="H13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="15"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="39"/>
+      <c r="M13" s="40"/>
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A14" s="3">
         <v>8</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="9" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="6" t="s">
+      <c r="G14" s="15"/>
+      <c r="H14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="15"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="39"/>
+      <c r="M14" s="40"/>
     </row>
     <row r="15" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A15" s="3">
@@ -1246,16 +1286,16 @@
         <v>27</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="8"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="10"/>
+      <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A16" s="3">
@@ -1273,16 +1313,16 @@
         <v>29</v>
       </c>
       <c r="G16" s="5"/>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="8"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="10"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A17" s="3">
@@ -1297,19 +1337,19 @@
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="8"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L17" s="7"/>
-      <c r="M17" s="8"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A18" s="3">
@@ -1327,43 +1367,43 @@
         <v>31</v>
       </c>
       <c r="G18" s="5"/>
-      <c r="H18" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="11" t="s">
+      <c r="H18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="10"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="15"/>
     </row>
     <row r="19" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A19" s="3">
         <v>13</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="9" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="9" t="s">
+      <c r="E19" s="15"/>
+      <c r="F19" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="6" t="s">
+      <c r="G19" s="15"/>
+      <c r="H19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="15"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="39"/>
+      <c r="M19" s="40"/>
     </row>
     <row r="20" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A20" s="3">
@@ -1381,16 +1421,16 @@
         <v>33</v>
       </c>
       <c r="G20" s="5"/>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L20" s="7"/>
-      <c r="M20" s="8"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="10"/>
+      <c r="M20" s="11"/>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A21" s="3">
@@ -1408,16 +1448,16 @@
         <v>36</v>
       </c>
       <c r="G21" s="5"/>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="8"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L21" s="10"/>
+      <c r="M21" s="11"/>
     </row>
     <row r="22" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A22" s="3">
@@ -1435,16 +1475,16 @@
         <v>51</v>
       </c>
       <c r="G22" s="5"/>
-      <c r="H22" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="8"/>
+      <c r="H22" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" s="10"/>
+      <c r="M22" s="11"/>
     </row>
     <row r="23" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A23" s="3">
@@ -1462,16 +1502,16 @@
         <v>51</v>
       </c>
       <c r="G23" s="5"/>
-      <c r="H23" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="11" t="s">
+      <c r="H23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L23" s="12"/>
-      <c r="M23" s="13"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A24" s="3">
@@ -1489,43 +1529,43 @@
         <v>50</v>
       </c>
       <c r="G24" s="5"/>
-      <c r="H24" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L24" s="7"/>
-      <c r="M24" s="8"/>
+      <c r="H24" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="10"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" s="10"/>
+      <c r="M24" s="11"/>
     </row>
     <row r="25" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A25" s="3">
         <v>19</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="9" t="s">
+      <c r="C25" s="15"/>
+      <c r="D25" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="9" t="s">
+      <c r="E25" s="15"/>
+      <c r="F25" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="6" t="s">
+      <c r="G25" s="15"/>
+      <c r="H25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L25" s="14"/>
-      <c r="M25" s="15"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L25" s="39"/>
+      <c r="M25" s="40"/>
     </row>
     <row r="26" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A26" s="3">
@@ -1543,16 +1583,16 @@
         <v>39</v>
       </c>
       <c r="G26" s="5"/>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I26" s="7"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L26" s="7"/>
-      <c r="M26" s="8"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L26" s="10"/>
+      <c r="M26" s="11"/>
     </row>
     <row r="27" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A27" s="3">
@@ -1570,16 +1610,16 @@
         <v>42</v>
       </c>
       <c r="G27" s="5"/>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L27" s="7"/>
-      <c r="M27" s="8"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L27" s="10"/>
+      <c r="M27" s="11"/>
     </row>
     <row r="28" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A28" s="3">
@@ -1597,16 +1637,16 @@
         <v>56</v>
       </c>
       <c r="G28" s="5"/>
-      <c r="H28" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="I28" s="12"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="11" t="s">
+      <c r="H28" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L28" s="12"/>
-      <c r="M28" s="13"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="8"/>
     </row>
     <row r="29" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A29" s="3">
@@ -1624,85 +1664,47 @@
         <v>56</v>
       </c>
       <c r="G29" s="5"/>
-      <c r="H29" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="11" t="s">
+      <c r="H29" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I29" s="7"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="13"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="131">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="K5:M6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:C6"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="H5:J6"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="D5:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="F21:G21"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="H18:J18"/>
@@ -1727,40 +1729,18 @@
     <mergeCell ref="K20:M20"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
@@ -1768,6 +1748,970 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="K14:M14"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="H5:J6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="K5:M6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:M15"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;11&amp;K000000 OFFICIAL</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24BF5C2E-C0F1-4148-BC9B-D3F85BAAF595}">
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="32.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="32.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="1"/>
+    <col min="9" max="9" width="24.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="9.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" style="1"/>
+    <col min="13" max="13" width="9" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="27">
+        <v>2</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="21">
+        <v>45827</v>
+      </c>
+      <c r="I3" s="22"/>
+      <c r="J3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="24"/>
+      <c r="L3" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="44"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="37"/>
+      <c r="H5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="13"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+    </row>
+    <row r="7" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A10" s="3">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A12" s="3">
+        <v>6</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="39"/>
+      <c r="M12" s="40"/>
+    </row>
+    <row r="13" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A13" s="3">
+        <v>7</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="39"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="39"/>
+      <c r="M13" s="40"/>
+    </row>
+    <row r="14" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A14" s="3">
+        <v>8</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="39"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="39"/>
+      <c r="M14" s="40"/>
+    </row>
+    <row r="15" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A15" s="3">
+        <v>9</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="10"/>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A16" s="3">
+        <v>10</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="10"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="42"/>
+      <c r="H17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="10"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A18" s="3">
+        <v>12</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="10"/>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="42"/>
+      <c r="F19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="10"/>
+      <c r="M19" s="11"/>
+    </row>
+    <row r="20" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="15"/>
+      <c r="F20" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="39"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="39"/>
+      <c r="M20" s="40"/>
+    </row>
+    <row r="21" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L21" s="10"/>
+      <c r="M21" s="11"/>
+    </row>
+    <row r="22" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L22" s="10"/>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A23" s="3"/>
+      <c r="B23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="10"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L23" s="10"/>
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A24" s="3"/>
+      <c r="B24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="10"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L24" s="10"/>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A25" s="3"/>
+      <c r="B25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="10"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L25" s="10"/>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="39"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L26" s="39"/>
+      <c r="M26" s="40"/>
+    </row>
+    <row r="27" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="B27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="10"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L27" s="10"/>
+      <c r="M27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A28" s="3"/>
+      <c r="B28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28" s="10"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L28" s="10"/>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="10"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L29" s="10"/>
+      <c r="M29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" s="4" customFormat="1" ht="60" customHeight="1">
+      <c r="A30" s="3"/>
+      <c r="B30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I30" s="10"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L30" s="10"/>
+      <c r="M30" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="136">
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="H5:J6"/>
+    <mergeCell ref="K5:M6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>